<commit_message>
messy commit. Don't care...
</commit_message>
<xml_diff>
--- a/source/cards/baralho_principal_DM_basic_set.xlsx
+++ b/source/cards/baralho_principal_DM_basic_set.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="61">
   <si>
     <t xml:space="preserve">qty</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
+    <t xml:space="preserve">set</t>
+  </si>
+  <si>
     <t xml:space="preserve">flavor</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO: FIX THIS SHIT</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -213,7 +219,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -235,13 +241,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -278,8 +297,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,13 +335,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
@@ -322,7 +349,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,60 +380,72 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>19</v>
+      <c r="F3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,28 +453,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>15</v>
+      <c r="J4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,28 +482,31 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>15</v>
+      <c r="J5" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,57 +514,63 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>15</v>
+      <c r="J6" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,28 +578,31 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>15</v>
+      <c r="J8" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,28 +610,31 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>15</v>
+      <c r="J9" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,57 +642,63 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>15</v>
+      <c r="J10" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>15</v>
+      <c r="J11" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,28 +706,31 @@
         <v>0</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>15</v>
+      <c r="J12" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,28 +738,31 @@
         <v>0</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>15</v>
+      <c r="J13" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,57 +770,63 @@
         <v>0</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>15</v>
+      <c r="J14" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,28 +834,31 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="0" t="s">
-        <v>15</v>
+      <c r="J16" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,28 +866,31 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>15</v>
+      <c r="J17" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,57 +898,63 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>15</v>
+      <c r="J18" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,28 +962,31 @@
         <v>0</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="0" t="s">
-        <v>15</v>
+      <c r="J20" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,28 +994,31 @@
         <v>0</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="0" t="s">
-        <v>15</v>
+      <c r="J21" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,57 +1026,63 @@
         <v>0</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>15</v>
+      <c r="J22" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,28 +1090,31 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>20</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="0" t="s">
-        <v>15</v>
+      <c r="J24" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,28 +1122,31 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>15</v>
+      <c r="J25" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,86 +1154,95 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="0" t="s">
-        <v>15</v>
+      <c r="J26" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,62 +1250,71 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>33</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="0" t="s">
-        <v>15</v>
+      <c r="J29" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="G31" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,28 +1322,31 @@
         <v>0</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,28 +1354,31 @@
         <v>0</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,28 +1386,31 @@
         <v>0</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,28 +1418,31 @@
         <v>0</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,217 +1450,253 @@
         <v>0</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="107.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="107.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="E39" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I38" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="119.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="I39" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="119.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I39" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I40" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="H40" s="0" t="s">
+      <c r="J40" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="60.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I40" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="178.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H41" s="0" t="s">
+      <c r="G41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="178.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I41" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="119.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H42" s="0" t="s">
+      <c r="G42" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="119.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I42" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H43" s="0" t="s">
+      <c r="G43" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="60.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I43" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H44" s="0" t="s">
+      <c r="G44" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="154.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I44" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="0" t="s">
+      <c r="G45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="I45" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J45" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,22 +1704,51 @@
         <v>2</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E46" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="G46" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="J46" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="I46" s="0" t="s">
-        <v>15</v>
+      <c r="F47" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>